<commit_message>
updated Bio and CCUS models with latest versions
</commit_message>
<xml_diff>
--- a/mppsteel/data/import_data/Bio Model.xlsx
+++ b/mppsteel/data/import_data/Bio Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://systemiq.sharepoint.com/Projects/MPP0006/Shared Documents/6_ Working documents/03 Steel python model/Data Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{79D791AD-293F-4810-B31E-95D2BFE39FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A66EE5A-8D6A-404D-8DA1-A97778D25998}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{79D791AD-293F-4810-B31E-95D2BFE39FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7684B0FB-6EC6-4F89-AE9C-E81089145917}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{1F6397B8-2A63-4EA8-A261-95081B332291}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" activeTab="1" xr2:uid="{1F6397B8-2A63-4EA8-A261-95081B332291}"/>
   </bookViews>
   <sheets>
     <sheet name="Feedstock_Prices" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="53">
   <si>
     <t>Region</t>
   </si>
@@ -88,9 +88,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>Japan, South Korea, Taiwan</t>
-  </si>
-  <si>
     <t>South and central Americas</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>Southeast Asia</t>
   </si>
   <si>
-    <t>RoW</t>
-  </si>
-  <si>
     <t>Tab</t>
   </si>
   <si>
@@ -170,6 +164,36 @@
   </si>
   <si>
     <t>Biomass_constraint</t>
+  </si>
+  <si>
+    <t>Australia / Oceania</t>
+  </si>
+  <si>
+    <t>Caribbean</t>
+  </si>
+  <si>
+    <t>Central Asia</t>
+  </si>
+  <si>
+    <t>East Europe</t>
+  </si>
+  <si>
+    <t>Japan + South Korea + Taiwan</t>
+  </si>
+  <si>
+    <t>NAFTA</t>
+  </si>
+  <si>
+    <t>North Asia, e.g., China</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>South Asia</t>
+  </si>
+  <si>
+    <t>Western Europe</t>
   </si>
 </sst>
 </file>
@@ -521,17 +545,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6351F1-5ED3-4A8A-9759-B4B81F522C07}">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="I131" sqref="I131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="13.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.46875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.76171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.17578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -560,7 +590,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -575,21 +605,21 @@
         <v>7</v>
       </c>
       <c r="F2">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="G2">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="H2">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="I2">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -604,21 +634,21 @@
         <v>7</v>
       </c>
       <c r="F3">
-        <v>10.93907237554669</v>
+        <v>10.9</v>
       </c>
       <c r="G3">
-        <v>10.93907237554669</v>
+        <v>10.9</v>
       </c>
       <c r="H3">
-        <v>10.93907237554669</v>
+        <v>10.9</v>
       </c>
       <c r="I3">
-        <v>10.93907237554669</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -633,21 +663,21 @@
         <v>7</v>
       </c>
       <c r="F4">
-        <v>6.8838354914252644</v>
+        <v>6.9</v>
       </c>
       <c r="G4">
-        <v>6.8838354914252644</v>
+        <v>6.9</v>
       </c>
       <c r="H4">
-        <v>6.8838354914252644</v>
+        <v>6.9</v>
       </c>
       <c r="I4">
-        <v>6.8838354914252644</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -662,21 +692,21 @@
         <v>7</v>
       </c>
       <c r="F5">
-        <v>7.6899696048632222</v>
+        <v>7.7</v>
       </c>
       <c r="G5">
-        <v>7.6899696048632222</v>
+        <v>7.7</v>
       </c>
       <c r="H5">
-        <v>7.6899696048632222</v>
+        <v>7.7</v>
       </c>
       <c r="I5">
-        <v>7.6899696048632222</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -691,21 +721,21 @@
         <v>7</v>
       </c>
       <c r="F6">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="G6">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="H6">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="I6">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
@@ -720,21 +750,21 @@
         <v>7</v>
       </c>
       <c r="F7">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="G7">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="H7">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="I7">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
@@ -749,21 +779,21 @@
         <v>7</v>
       </c>
       <c r="F8">
-        <v>11.002209554595909</v>
+        <v>11</v>
       </c>
       <c r="G8">
-        <v>10.387052459116466</v>
+        <v>10.4</v>
       </c>
       <c r="H8">
-        <v>9.8960555113484734</v>
+        <v>9.9</v>
       </c>
       <c r="I8">
-        <v>9.4950746706712774</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -778,21 +808,21 @@
         <v>7</v>
       </c>
       <c r="F9">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="G9">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="H9">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="I9">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -807,21 +837,21 @@
         <v>7</v>
       </c>
       <c r="F10">
-        <v>5.7249999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="G10">
-        <v>5.7249999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="H10">
-        <v>5.7249999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="I10">
-        <v>5.7249999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -836,21 +866,21 @@
         <v>7</v>
       </c>
       <c r="F11">
-        <v>6.3154002392841999</v>
+        <v>6.3</v>
       </c>
       <c r="G11">
-        <v>6.3154002392841999</v>
+        <v>6.3</v>
       </c>
       <c r="H11">
-        <v>6.3154002392841999</v>
+        <v>6.3</v>
       </c>
       <c r="I11">
-        <v>6.3154002392841999</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -865,21 +895,21 @@
         <v>7</v>
       </c>
       <c r="F12">
-        <v>3.0300000000000002</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>3.0300000000000002</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <v>3.0300000000000002</v>
+        <v>3</v>
       </c>
       <c r="I12">
-        <v>3.0300000000000002</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -894,21 +924,21 @@
         <v>7</v>
       </c>
       <c r="F13">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="G13">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="H13">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="I13">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -923,21 +953,21 @@
         <v>7</v>
       </c>
       <c r="F14">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="G14">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="H14">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="I14">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
@@ -952,21 +982,21 @@
         <v>7</v>
       </c>
       <c r="F15">
-        <v>9.7918423469547964</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G15">
-        <v>8.7332788993614709</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="H15">
-        <v>7.8883704595392743</v>
+        <v>7.9</v>
       </c>
       <c r="I15">
-        <v>7.1983619003511459</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -981,21 +1011,21 @@
         <v>7</v>
       </c>
       <c r="F16">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="G16">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="H16">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="I16">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -1010,21 +1040,21 @@
         <v>7</v>
       </c>
       <c r="F17">
-        <v>5.4601600000000001</v>
+        <v>5.5</v>
       </c>
       <c r="G17">
-        <v>5.4601600000000001</v>
+        <v>5.5</v>
       </c>
       <c r="H17">
-        <v>5.4601600000000001</v>
+        <v>5.5</v>
       </c>
       <c r="I17">
-        <v>5.4601600000000001</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -1039,21 +1069,21 @@
         <v>7</v>
       </c>
       <c r="F18">
-        <v>13.684060292637488</v>
+        <v>13.7</v>
       </c>
       <c r="G18">
-        <v>13.684060292637488</v>
+        <v>13.7</v>
       </c>
       <c r="H18">
-        <v>13.684060292637488</v>
+        <v>13.7</v>
       </c>
       <c r="I18">
-        <v>13.684060292637488</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -1068,21 +1098,21 @@
         <v>7</v>
       </c>
       <c r="F19">
-        <v>2.8328787010506211</v>
+        <v>2.8</v>
       </c>
       <c r="G19">
-        <v>2.8328787010506211</v>
+        <v>2.8</v>
       </c>
       <c r="H19">
-        <v>2.8328787010506211</v>
+        <v>2.8</v>
       </c>
       <c r="I19">
-        <v>2.8328787010506211</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
@@ -1097,21 +1127,21 @@
         <v>7</v>
       </c>
       <c r="F20">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="G20">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="H20">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="I20">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -1126,21 +1156,21 @@
         <v>7</v>
       </c>
       <c r="F21">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="G21">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="H21">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="I21">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -1155,21 +1185,21 @@
         <v>7</v>
       </c>
       <c r="F22">
-        <v>13.540148373563634</v>
+        <v>13.5</v>
       </c>
       <c r="G22">
-        <v>12.069084392971984</v>
+        <v>12.1</v>
       </c>
       <c r="H22">
-        <v>10.894932408463053</v>
+        <v>10.9</v>
       </c>
       <c r="I22">
-        <v>9.9360416211140929</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>16</v>
@@ -1184,21 +1214,21 @@
         <v>7</v>
       </c>
       <c r="F23">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="G23">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="H23">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="I23">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>16</v>
@@ -1213,21 +1243,21 @@
         <v>7</v>
       </c>
       <c r="F24">
-        <v>4.8320000000000007</v>
+        <v>4.8</v>
       </c>
       <c r="G24">
-        <v>4.8320000000000007</v>
+        <v>4.8</v>
       </c>
       <c r="H24">
-        <v>4.8320000000000007</v>
+        <v>4.8</v>
       </c>
       <c r="I24">
-        <v>4.8320000000000007</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>16</v>
@@ -1242,21 +1272,21 @@
         <v>7</v>
       </c>
       <c r="F25">
-        <v>12.673510362262286</v>
+        <v>12.7</v>
       </c>
       <c r="G25">
-        <v>12.673510362262286</v>
+        <v>12.7</v>
       </c>
       <c r="H25">
-        <v>12.673510362262286</v>
+        <v>12.7</v>
       </c>
       <c r="I25">
-        <v>12.673510362262286</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>16</v>
@@ -1271,21 +1301,21 @@
         <v>7</v>
       </c>
       <c r="F26">
-        <v>1.9227828746177369</v>
+        <v>1.9</v>
       </c>
       <c r="G26">
-        <v>1.9227828746177369</v>
+        <v>1.9</v>
       </c>
       <c r="H26">
-        <v>1.9227828746177369</v>
+        <v>1.9</v>
       </c>
       <c r="I26">
-        <v>1.9227828746177369</v>
+        <v>1.9</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
         <v>16</v>
@@ -1300,21 +1330,21 @@
         <v>7</v>
       </c>
       <c r="F27">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="G27">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="H27">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="I27">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
         <v>16</v>
@@ -1329,21 +1359,21 @@
         <v>7</v>
       </c>
       <c r="F28">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="G28">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="H28">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="I28">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
         <v>16</v>
@@ -1358,21 +1388,21 @@
         <v>7</v>
       </c>
       <c r="F29">
-        <v>12.882267966739867</v>
+        <v>12.9</v>
       </c>
       <c r="G29">
-        <v>11.386055105694036</v>
+        <v>11.4</v>
       </c>
       <c r="H29">
-        <v>10.191830161556538</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="I29">
-        <v>9.2165464571775804</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
         <v>17</v>
@@ -1387,21 +1417,21 @@
         <v>7</v>
       </c>
       <c r="F30">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="G30">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="H30">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="I30">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
@@ -1416,21 +1446,21 @@
         <v>7</v>
       </c>
       <c r="F31">
-        <v>5.4601600000000001</v>
+        <v>5.7</v>
       </c>
       <c r="G31">
-        <v>5.4601600000000001</v>
+        <v>5.7</v>
       </c>
       <c r="H31">
-        <v>5.4601600000000001</v>
+        <v>5.7</v>
       </c>
       <c r="I31">
-        <v>5.4601600000000001</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
@@ -1445,21 +1475,21 @@
         <v>7</v>
       </c>
       <c r="F32">
-        <v>13.684060292637488</v>
+        <v>6.3</v>
       </c>
       <c r="G32">
-        <v>13.684060292637488</v>
+        <v>6.3</v>
       </c>
       <c r="H32">
-        <v>13.684060292637488</v>
+        <v>6.3</v>
       </c>
       <c r="I32">
-        <v>13.684060292637488</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
         <v>17</v>
@@ -1474,21 +1504,21 @@
         <v>7</v>
       </c>
       <c r="F33">
-        <v>2.8328787010506211</v>
+        <v>3</v>
       </c>
       <c r="G33">
-        <v>2.8328787010506211</v>
+        <v>3</v>
       </c>
       <c r="H33">
-        <v>2.8328787010506211</v>
+        <v>3</v>
       </c>
       <c r="I33">
-        <v>2.8328787010506211</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
         <v>17</v>
@@ -1503,21 +1533,21 @@
         <v>7</v>
       </c>
       <c r="F34">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="G34">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="H34">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="I34">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B35" t="s">
         <v>17</v>
@@ -1532,21 +1562,21 @@
         <v>7</v>
       </c>
       <c r="F35">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="G35">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="H35">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="I35">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
@@ -1561,24 +1591,24 @@
         <v>7</v>
       </c>
       <c r="F36">
-        <v>13.540148373563634</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G36">
-        <v>12.069084392971984</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="H36">
-        <v>10.894932408463053</v>
+        <v>7.9</v>
       </c>
       <c r="I36">
-        <v>9.9360416211140929</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1590,24 +1620,24 @@
         <v>7</v>
       </c>
       <c r="F37">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="G37">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="H37">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="I37">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B38" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -1619,24 +1649,24 @@
         <v>7</v>
       </c>
       <c r="F38">
-        <v>5.7249999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="G38">
-        <v>5.7249999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="H38">
-        <v>5.7249999999999996</v>
+        <v>5.7</v>
       </c>
       <c r="I38">
-        <v>5.7249999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -1648,24 +1678,24 @@
         <v>7</v>
       </c>
       <c r="F39">
-        <v>6.3154002392841999</v>
+        <v>6.3</v>
       </c>
       <c r="G39">
-        <v>6.3154002392841999</v>
+        <v>6.3</v>
       </c>
       <c r="H39">
-        <v>6.3154002392841999</v>
+        <v>6.3</v>
       </c>
       <c r="I39">
-        <v>6.3154002392841999</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1677,24 +1707,24 @@
         <v>7</v>
       </c>
       <c r="F40">
-        <v>3.0300000000000002</v>
+        <v>3</v>
       </c>
       <c r="G40">
-        <v>3.0300000000000002</v>
+        <v>3</v>
       </c>
       <c r="H40">
-        <v>3.0300000000000002</v>
+        <v>3</v>
       </c>
       <c r="I40">
-        <v>3.0300000000000002</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1706,24 +1736,24 @@
         <v>7</v>
       </c>
       <c r="F41">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="G41">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="H41">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="I41">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1735,24 +1765,24 @@
         <v>7</v>
       </c>
       <c r="F42">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="G42">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="H42">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="I42">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -1764,24 +1794,24 @@
         <v>7</v>
       </c>
       <c r="F43">
-        <v>9.7918423469547964</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="G43">
-        <v>8.7332788993614709</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="H43">
-        <v>7.8883704595392743</v>
+        <v>7.9</v>
       </c>
       <c r="I43">
-        <v>7.1983619003511459</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -1793,24 +1823,24 @@
         <v>7</v>
       </c>
       <c r="F44">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="G44">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="H44">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
       <c r="I44">
-        <v>20.967413442757557</v>
+        <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1822,24 +1852,24 @@
         <v>7</v>
       </c>
       <c r="F45">
-        <v>10.93907237554669</v>
+        <v>5.7</v>
       </c>
       <c r="G45">
-        <v>10.93907237554669</v>
+        <v>5.7</v>
       </c>
       <c r="H45">
-        <v>10.93907237554669</v>
+        <v>5.7</v>
       </c>
       <c r="I45">
-        <v>10.93907237554669</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1851,24 +1881,24 @@
         <v>7</v>
       </c>
       <c r="F46">
-        <v>6.8838354914252644</v>
+        <v>6.3</v>
       </c>
       <c r="G46">
-        <v>6.8838354914252644</v>
+        <v>6.3</v>
       </c>
       <c r="H46">
-        <v>6.8838354914252644</v>
+        <v>6.3</v>
       </c>
       <c r="I46">
-        <v>6.8838354914252644</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1880,24 +1910,24 @@
         <v>7</v>
       </c>
       <c r="F47">
-        <v>7.6899696048632222</v>
+        <v>3</v>
       </c>
       <c r="G47">
-        <v>7.6899696048632222</v>
+        <v>3</v>
       </c>
       <c r="H47">
-        <v>7.6899696048632222</v>
+        <v>3</v>
       </c>
       <c r="I47">
-        <v>7.6899696048632222</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B48" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1909,24 +1939,24 @@
         <v>7</v>
       </c>
       <c r="F48">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="G48">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="H48">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
       <c r="I48">
-        <v>13.108108108108109</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B49" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1938,857 +1968,2104 @@
         <v>7</v>
       </c>
       <c r="F49">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="G49">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="H49">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
       <c r="I49">
-        <v>36.423841059602651</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E50" t="s">
         <v>7</v>
       </c>
       <c r="F50">
-        <v>11.002209554595909</v>
+        <v>21</v>
       </c>
       <c r="G50">
-        <v>10.387052459116466</v>
+        <v>21</v>
       </c>
       <c r="H50">
-        <v>9.8960555113484734</v>
+        <v>21</v>
       </c>
       <c r="I50">
-        <v>9.4950746706712774</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B51" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E51" t="s">
         <v>7</v>
       </c>
       <c r="F51">
-        <v>20.967413442757557</v>
+        <v>5.7</v>
       </c>
       <c r="G51">
-        <v>20.967413442757557</v>
+        <v>5.7</v>
       </c>
       <c r="H51">
-        <v>20.967413442757557</v>
+        <v>5.7</v>
       </c>
       <c r="I51">
-        <v>20.967413442757557</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E52" t="s">
         <v>7</v>
       </c>
       <c r="F52">
-        <v>5.7249999999999996</v>
+        <v>6.3</v>
       </c>
       <c r="G52">
-        <v>5.7249999999999996</v>
+        <v>6.3</v>
       </c>
       <c r="H52">
-        <v>5.7249999999999996</v>
+        <v>6.3</v>
       </c>
       <c r="I52">
-        <v>5.7249999999999996</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E53" t="s">
         <v>7</v>
       </c>
       <c r="F53">
-        <v>6.3154002392841999</v>
+        <v>3</v>
       </c>
       <c r="G53">
-        <v>6.3154002392841999</v>
+        <v>3</v>
       </c>
       <c r="H53">
-        <v>6.3154002392841999</v>
+        <v>3</v>
       </c>
       <c r="I53">
-        <v>6.3154002392841999</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E54" t="s">
         <v>7</v>
       </c>
       <c r="F54">
-        <v>3.0300000000000002</v>
+        <v>13.1</v>
       </c>
       <c r="G54">
-        <v>3.0300000000000002</v>
+        <v>13.1</v>
       </c>
       <c r="H54">
-        <v>3.0300000000000002</v>
+        <v>13.1</v>
       </c>
       <c r="I54">
-        <v>3.0300000000000002</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E55" t="s">
         <v>7</v>
       </c>
       <c r="F55">
-        <v>13.108108108108109</v>
+        <v>36.4</v>
       </c>
       <c r="G55">
-        <v>13.108108108108109</v>
+        <v>36.4</v>
       </c>
       <c r="H55">
-        <v>13.108108108108109</v>
+        <v>36.4</v>
       </c>
       <c r="I55">
-        <v>13.108108108108109</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C56" t="s">
         <v>5</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E56" t="s">
         <v>7</v>
       </c>
       <c r="F56">
-        <v>36.423841059602651</v>
+        <v>21</v>
       </c>
       <c r="G56">
-        <v>36.423841059602651</v>
+        <v>21</v>
       </c>
       <c r="H56">
-        <v>36.423841059602651</v>
+        <v>21</v>
       </c>
       <c r="I56">
-        <v>36.423841059602651</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A57" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
         <v>5</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
       </c>
       <c r="F57">
-        <v>9.7918423469547964</v>
+        <v>5.5</v>
       </c>
       <c r="G57">
-        <v>8.7332788993614709</v>
+        <v>5.5</v>
       </c>
       <c r="H57">
-        <v>7.8883704595392743</v>
+        <v>5.5</v>
       </c>
       <c r="I57">
-        <v>7.1983619003511459</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B58" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C58" t="s">
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E58" t="s">
         <v>7</v>
       </c>
       <c r="F58">
-        <v>20.967413442757557</v>
+        <v>13.7</v>
       </c>
       <c r="G58">
-        <v>20.967413442757557</v>
+        <v>13.7</v>
       </c>
       <c r="H58">
-        <v>20.967413442757557</v>
+        <v>13.7</v>
       </c>
       <c r="I58">
-        <v>20.967413442757557</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A59" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E59" t="s">
         <v>7</v>
       </c>
       <c r="F59">
-        <v>10.93907237554669</v>
+        <v>2.8</v>
       </c>
       <c r="G59">
-        <v>10.93907237554669</v>
+        <v>2.8</v>
       </c>
       <c r="H59">
-        <v>10.93907237554669</v>
+        <v>2.8</v>
       </c>
       <c r="I59">
-        <v>10.93907237554669</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A60" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C60" t="s">
         <v>5</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E60" t="s">
         <v>7</v>
       </c>
       <c r="F60">
-        <v>6.8838354914252644</v>
+        <v>13.1</v>
       </c>
       <c r="G60">
-        <v>6.8838354914252644</v>
+        <v>13.1</v>
       </c>
       <c r="H60">
-        <v>6.8838354914252644</v>
+        <v>13.1</v>
       </c>
       <c r="I60">
-        <v>6.8838354914252644</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E61" t="s">
         <v>7</v>
       </c>
       <c r="F61">
-        <v>7.6899696048632222</v>
+        <v>36.4</v>
       </c>
       <c r="G61">
-        <v>7.6899696048632222</v>
+        <v>36.4</v>
       </c>
       <c r="H61">
-        <v>7.6899696048632222</v>
+        <v>36.4</v>
       </c>
       <c r="I61">
-        <v>7.6899696048632222</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A62" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E62" t="s">
         <v>7</v>
       </c>
       <c r="F62">
-        <v>13.108108108108109</v>
+        <v>21</v>
       </c>
       <c r="G62">
-        <v>13.108108108108109</v>
+        <v>21</v>
       </c>
       <c r="H62">
-        <v>13.108108108108109</v>
+        <v>21</v>
       </c>
       <c r="I62">
-        <v>13.108108108108109</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A63" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C63" t="s">
         <v>5</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
       </c>
       <c r="F63">
-        <v>36.423841059602651</v>
+        <v>5.5</v>
       </c>
       <c r="G63">
-        <v>36.423841059602651</v>
+        <v>5.5</v>
       </c>
       <c r="H63">
-        <v>36.423841059602651</v>
+        <v>5.5</v>
       </c>
       <c r="I63">
-        <v>36.423841059602651</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E64" t="s">
         <v>7</v>
       </c>
       <c r="F64">
-        <v>11.002209554595909</v>
+        <v>13.7</v>
       </c>
       <c r="G64">
-        <v>10.387052459116466</v>
+        <v>13.7</v>
       </c>
       <c r="H64">
-        <v>9.8960555113484734</v>
+        <v>13.7</v>
       </c>
       <c r="I64">
-        <v>9.4950746706712774</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B65" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="D65" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E65" t="s">
         <v>7</v>
       </c>
       <c r="F65">
-        <v>20.967413442757557</v>
+        <v>2.8</v>
       </c>
       <c r="G65">
-        <v>20.967413442757557</v>
+        <v>2.8</v>
       </c>
       <c r="H65">
-        <v>20.967413442757557</v>
+        <v>2.8</v>
       </c>
       <c r="I65">
-        <v>20.967413442757557</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B66" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C66" t="s">
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E66" t="s">
         <v>7</v>
       </c>
       <c r="F66">
-        <v>5.4601600000000001</v>
+        <v>13.1</v>
       </c>
       <c r="G66">
-        <v>5.4601600000000001</v>
+        <v>13.1</v>
       </c>
       <c r="H66">
-        <v>5.4601600000000001</v>
+        <v>13.1</v>
       </c>
       <c r="I66">
-        <v>5.4601600000000001</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B67" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C67" t="s">
         <v>5</v>
       </c>
       <c r="D67" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E67" t="s">
         <v>7</v>
       </c>
       <c r="F67">
-        <v>13.684060292637488</v>
+        <v>36.4</v>
       </c>
       <c r="G67">
-        <v>13.684060292637488</v>
+        <v>36.4</v>
       </c>
       <c r="H67">
-        <v>13.684060292637488</v>
+        <v>36.4</v>
       </c>
       <c r="I67">
-        <v>13.684060292637488</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A68" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B68" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
       </c>
       <c r="D68" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E68" t="s">
         <v>7</v>
       </c>
       <c r="F68">
-        <v>2.8328787010506211</v>
+        <v>21</v>
       </c>
       <c r="G68">
-        <v>2.8328787010506211</v>
+        <v>21</v>
       </c>
       <c r="H68">
-        <v>2.8328787010506211</v>
+        <v>21</v>
       </c>
       <c r="I68">
-        <v>2.8328787010506211</v>
+        <v>21</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B69" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E69" t="s">
         <v>7</v>
       </c>
       <c r="F69">
-        <v>13.108108108108109</v>
+        <v>10.9</v>
       </c>
       <c r="G69">
-        <v>13.108108108108109</v>
+        <v>10.9</v>
       </c>
       <c r="H69">
-        <v>13.108108108108109</v>
+        <v>10.9</v>
       </c>
       <c r="I69">
-        <v>13.108108108108109</v>
+        <v>10.9</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B70" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E70" t="s">
         <v>7</v>
       </c>
       <c r="F70">
-        <v>36.423841059602651</v>
+        <v>6.9</v>
       </c>
       <c r="G70">
-        <v>36.423841059602651</v>
+        <v>6.9</v>
       </c>
       <c r="H70">
-        <v>36.423841059602651</v>
+        <v>6.9</v>
       </c>
       <c r="I70">
-        <v>36.423841059602651</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A71" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B71" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E71" t="s">
         <v>7</v>
       </c>
       <c r="F71">
-        <v>13.540148373563634</v>
+        <v>7.7</v>
       </c>
       <c r="G71">
-        <v>12.069084392971984</v>
+        <v>7.7</v>
       </c>
       <c r="H71">
-        <v>10.894932408463053</v>
+        <v>7.7</v>
       </c>
       <c r="I71">
-        <v>9.9360416211140929</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B72" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C72" t="s">
         <v>5</v>
       </c>
       <c r="D72" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E72" t="s">
         <v>7</v>
       </c>
       <c r="F72">
-        <v>20.967413442757557</v>
+        <v>13.1</v>
       </c>
       <c r="G72">
-        <v>20.967413442757557</v>
+        <v>13.1</v>
       </c>
       <c r="H72">
-        <v>20.967413442757557</v>
+        <v>13.1</v>
       </c>
       <c r="I72">
-        <v>20.967413442757557</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A73" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B73" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
         <v>7</v>
       </c>
       <c r="F73">
-        <v>6.7390580938866727</v>
+        <v>36.4</v>
       </c>
       <c r="G73">
-        <v>6.7390580938866727</v>
+        <v>36.4</v>
       </c>
       <c r="H73">
-        <v>6.7390580938866727</v>
+        <v>36.4</v>
       </c>
       <c r="I73">
-        <v>6.7390580938866727</v>
+        <v>36.4</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A74" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B74" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E74" t="s">
         <v>7</v>
       </c>
       <c r="F74">
-        <v>9.8892015964023088</v>
+        <v>21</v>
       </c>
       <c r="G74">
-        <v>9.8892015964023088</v>
+        <v>21</v>
       </c>
       <c r="H74">
-        <v>9.8892015964023088</v>
+        <v>21</v>
       </c>
       <c r="I74">
-        <v>9.8892015964023088</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A75" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B75" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
       </c>
       <c r="D75" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E75" t="s">
         <v>7</v>
       </c>
       <c r="F75">
-        <v>3.8689077951328952</v>
+        <v>5.5</v>
       </c>
       <c r="G75">
-        <v>3.8689077951328952</v>
+        <v>5.5</v>
       </c>
       <c r="H75">
-        <v>3.8689077951328952</v>
+        <v>5.5</v>
       </c>
       <c r="I75">
-        <v>3.8689077951328952</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B76" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C76" t="s">
         <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E76" t="s">
         <v>7</v>
       </c>
       <c r="F76">
-        <v>13.108108108108109</v>
+        <v>13.7</v>
       </c>
       <c r="G76">
-        <v>13.108108108108109</v>
+        <v>13.7</v>
       </c>
       <c r="H76">
-        <v>13.108108108108109</v>
+        <v>13.7</v>
       </c>
       <c r="I76">
-        <v>13.108108108108109</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A77" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B77" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
       </c>
       <c r="D77" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E77" t="s">
         <v>7</v>
       </c>
       <c r="F77">
-        <v>36.423841059602651</v>
+        <v>2.8</v>
       </c>
       <c r="G77">
-        <v>36.423841059602651</v>
+        <v>2.8</v>
       </c>
       <c r="H77">
-        <v>36.423841059602651</v>
+        <v>2.8</v>
       </c>
       <c r="I77">
-        <v>36.423841059602651</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A78" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B78" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C78" t="s">
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E78" t="s">
         <v>7</v>
       </c>
       <c r="F78">
-        <v>11.804117060463552</v>
+        <v>13.1</v>
       </c>
       <c r="G78">
-        <v>10.643867714285989</v>
+        <v>13.1</v>
       </c>
       <c r="H78">
-        <v>9.7177971352268351</v>
+        <v>13.1</v>
       </c>
       <c r="I78">
-        <v>8.9615061623285239</v>
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A79" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" t="s">
+        <v>47</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" t="s">
+        <v>7</v>
+      </c>
+      <c r="F79">
+        <v>36.4</v>
+      </c>
+      <c r="G79">
+        <v>36.4</v>
+      </c>
+      <c r="H79">
+        <v>36.4</v>
+      </c>
+      <c r="I79">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A80" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" t="s">
+        <v>7</v>
+      </c>
+      <c r="F80">
+        <v>21</v>
+      </c>
+      <c r="G80">
+        <v>21</v>
+      </c>
+      <c r="H80">
+        <v>21</v>
+      </c>
+      <c r="I80">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A81" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" t="s">
+        <v>7</v>
+      </c>
+      <c r="F81">
+        <v>5.7</v>
+      </c>
+      <c r="G81">
+        <v>5.7</v>
+      </c>
+      <c r="H81">
+        <v>5.7</v>
+      </c>
+      <c r="I81">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A82" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s">
+        <v>7</v>
+      </c>
+      <c r="F82">
+        <v>6.3</v>
+      </c>
+      <c r="G82">
+        <v>6.3</v>
+      </c>
+      <c r="H82">
+        <v>6.3</v>
+      </c>
+      <c r="I82">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A83" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83">
+        <v>3</v>
+      </c>
+      <c r="G83">
+        <v>3</v>
+      </c>
+      <c r="H83">
+        <v>3</v>
+      </c>
+      <c r="I83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84">
+        <v>13.1</v>
+      </c>
+      <c r="G84">
+        <v>13.1</v>
+      </c>
+      <c r="H84">
+        <v>13.1</v>
+      </c>
+      <c r="I84">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A85" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" t="s">
+        <v>7</v>
+      </c>
+      <c r="F85">
+        <v>36.4</v>
+      </c>
+      <c r="G85">
+        <v>36.4</v>
+      </c>
+      <c r="H85">
+        <v>36.4</v>
+      </c>
+      <c r="I85">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A86" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" t="s">
+        <v>48</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" t="s">
+        <v>7</v>
+      </c>
+      <c r="F86">
+        <v>21</v>
+      </c>
+      <c r="G86">
+        <v>21</v>
+      </c>
+      <c r="H86">
+        <v>21</v>
+      </c>
+      <c r="I86">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A87" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" t="s">
+        <v>48</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" t="s">
+        <v>7</v>
+      </c>
+      <c r="F87">
+        <v>5.7</v>
+      </c>
+      <c r="G87">
+        <v>5.7</v>
+      </c>
+      <c r="H87">
+        <v>5.7</v>
+      </c>
+      <c r="I87">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A88" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" t="s">
+        <v>48</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" t="s">
+        <v>7</v>
+      </c>
+      <c r="F88">
+        <v>6.3</v>
+      </c>
+      <c r="G88">
+        <v>6.3</v>
+      </c>
+      <c r="H88">
+        <v>6.3</v>
+      </c>
+      <c r="I88">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A89" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" t="s">
+        <v>48</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" t="s">
+        <v>7</v>
+      </c>
+      <c r="F89">
+        <v>3</v>
+      </c>
+      <c r="G89">
+        <v>3</v>
+      </c>
+      <c r="H89">
+        <v>3</v>
+      </c>
+      <c r="I89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A90" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" t="s">
+        <v>48</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" t="s">
+        <v>7</v>
+      </c>
+      <c r="F90">
+        <v>13.1</v>
+      </c>
+      <c r="G90">
+        <v>13.1</v>
+      </c>
+      <c r="H90">
+        <v>13.1</v>
+      </c>
+      <c r="I90">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A91" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" t="s">
+        <v>48</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" t="s">
+        <v>7</v>
+      </c>
+      <c r="F91">
+        <v>36.4</v>
+      </c>
+      <c r="G91">
+        <v>36.4</v>
+      </c>
+      <c r="H91">
+        <v>36.4</v>
+      </c>
+      <c r="I91">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A92" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" t="s">
+        <v>49</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" t="s">
+        <v>7</v>
+      </c>
+      <c r="F92">
+        <v>21</v>
+      </c>
+      <c r="G92">
+        <v>21</v>
+      </c>
+      <c r="H92">
+        <v>21</v>
+      </c>
+      <c r="I92">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A93" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" t="s">
+        <v>49</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93">
+        <v>5.5</v>
+      </c>
+      <c r="G93">
+        <v>5.5</v>
+      </c>
+      <c r="H93">
+        <v>5.5</v>
+      </c>
+      <c r="I93">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A94" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" t="s">
+        <v>49</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>7</v>
+      </c>
+      <c r="F94">
+        <v>13.7</v>
+      </c>
+      <c r="G94">
+        <v>13.7</v>
+      </c>
+      <c r="H94">
+        <v>13.7</v>
+      </c>
+      <c r="I94">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A95" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" t="s">
+        <v>49</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D95" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95" t="s">
+        <v>7</v>
+      </c>
+      <c r="F95">
+        <v>2.8</v>
+      </c>
+      <c r="G95">
+        <v>2.8</v>
+      </c>
+      <c r="H95">
+        <v>2.8</v>
+      </c>
+      <c r="I95">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A96" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" t="s">
+        <v>49</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" t="s">
+        <v>11</v>
+      </c>
+      <c r="E96" t="s">
+        <v>7</v>
+      </c>
+      <c r="F96">
+        <v>13.1</v>
+      </c>
+      <c r="G96">
+        <v>13.1</v>
+      </c>
+      <c r="H96">
+        <v>13.1</v>
+      </c>
+      <c r="I96">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A97" t="s">
+        <v>23</v>
+      </c>
+      <c r="B97" t="s">
+        <v>49</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97" t="s">
+        <v>7</v>
+      </c>
+      <c r="F97">
+        <v>36.4</v>
+      </c>
+      <c r="G97">
+        <v>36.4</v>
+      </c>
+      <c r="H97">
+        <v>36.4</v>
+      </c>
+      <c r="I97">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A98" t="s">
+        <v>23</v>
+      </c>
+      <c r="B98" t="s">
+        <v>50</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" t="s">
+        <v>7</v>
+      </c>
+      <c r="F98">
+        <v>21</v>
+      </c>
+      <c r="G98">
+        <v>21</v>
+      </c>
+      <c r="H98">
+        <v>21</v>
+      </c>
+      <c r="I98">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A99" t="s">
+        <v>23</v>
+      </c>
+      <c r="B99" t="s">
+        <v>50</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" t="s">
+        <v>7</v>
+      </c>
+      <c r="F99">
+        <v>10.9</v>
+      </c>
+      <c r="G99">
+        <v>10.9</v>
+      </c>
+      <c r="H99">
+        <v>10.9</v>
+      </c>
+      <c r="I99">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A100" t="s">
+        <v>23</v>
+      </c>
+      <c r="B100" t="s">
+        <v>50</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" t="s">
+        <v>7</v>
+      </c>
+      <c r="F100">
+        <v>6.9</v>
+      </c>
+      <c r="G100">
+        <v>6.9</v>
+      </c>
+      <c r="H100">
+        <v>6.9</v>
+      </c>
+      <c r="I100">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A101" t="s">
+        <v>23</v>
+      </c>
+      <c r="B101" t="s">
+        <v>50</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+      <c r="D101" t="s">
+        <v>10</v>
+      </c>
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+      <c r="F101">
+        <v>7.7</v>
+      </c>
+      <c r="G101">
+        <v>7.7</v>
+      </c>
+      <c r="H101">
+        <v>7.7</v>
+      </c>
+      <c r="I101">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A102" t="s">
+        <v>23</v>
+      </c>
+      <c r="B102" t="s">
+        <v>50</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" t="s">
+        <v>7</v>
+      </c>
+      <c r="F102">
+        <v>13.1</v>
+      </c>
+      <c r="G102">
+        <v>13.1</v>
+      </c>
+      <c r="H102">
+        <v>13.1</v>
+      </c>
+      <c r="I102">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A103" t="s">
+        <v>23</v>
+      </c>
+      <c r="B103" t="s">
+        <v>50</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+      <c r="D103" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" t="s">
+        <v>7</v>
+      </c>
+      <c r="F103">
+        <v>36.4</v>
+      </c>
+      <c r="G103">
+        <v>36.4</v>
+      </c>
+      <c r="H103">
+        <v>36.4</v>
+      </c>
+      <c r="I103">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A104" t="s">
+        <v>23</v>
+      </c>
+      <c r="B104" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104">
+        <v>21</v>
+      </c>
+      <c r="G104">
+        <v>21</v>
+      </c>
+      <c r="H104">
+        <v>21</v>
+      </c>
+      <c r="I104">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A105" t="s">
+        <v>23</v>
+      </c>
+      <c r="B105" t="s">
+        <v>51</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" t="s">
+        <v>7</v>
+      </c>
+      <c r="F105">
+        <v>5.7</v>
+      </c>
+      <c r="G105">
+        <v>5.7</v>
+      </c>
+      <c r="H105">
+        <v>5.7</v>
+      </c>
+      <c r="I105">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A106" t="s">
+        <v>23</v>
+      </c>
+      <c r="B106" t="s">
+        <v>51</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" t="s">
+        <v>7</v>
+      </c>
+      <c r="F106">
+        <v>6.3</v>
+      </c>
+      <c r="G106">
+        <v>6.3</v>
+      </c>
+      <c r="H106">
+        <v>6.3</v>
+      </c>
+      <c r="I106">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A107" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" t="s">
+        <v>51</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" t="s">
+        <v>7</v>
+      </c>
+      <c r="F107">
+        <v>3</v>
+      </c>
+      <c r="G107">
+        <v>3</v>
+      </c>
+      <c r="H107">
+        <v>3</v>
+      </c>
+      <c r="I107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A108" t="s">
+        <v>23</v>
+      </c>
+      <c r="B108" t="s">
+        <v>51</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>11</v>
+      </c>
+      <c r="E108" t="s">
+        <v>7</v>
+      </c>
+      <c r="F108">
+        <v>13.1</v>
+      </c>
+      <c r="G108">
+        <v>13.1</v>
+      </c>
+      <c r="H108">
+        <v>13.1</v>
+      </c>
+      <c r="I108">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A109" t="s">
+        <v>23</v>
+      </c>
+      <c r="B109" t="s">
+        <v>51</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109" t="s">
+        <v>7</v>
+      </c>
+      <c r="F109">
+        <v>36.4</v>
+      </c>
+      <c r="G109">
+        <v>36.4</v>
+      </c>
+      <c r="H109">
+        <v>36.4</v>
+      </c>
+      <c r="I109">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A110" t="s">
+        <v>23</v>
+      </c>
+      <c r="B110" t="s">
+        <v>21</v>
+      </c>
+      <c r="C110" t="s">
+        <v>5</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" t="s">
+        <v>7</v>
+      </c>
+      <c r="F110">
+        <v>21</v>
+      </c>
+      <c r="G110">
+        <v>21</v>
+      </c>
+      <c r="H110">
+        <v>21</v>
+      </c>
+      <c r="I110">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A111" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" t="s">
+        <v>21</v>
+      </c>
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" t="s">
+        <v>7</v>
+      </c>
+      <c r="F111">
+        <v>5.5</v>
+      </c>
+      <c r="G111">
+        <v>5.5</v>
+      </c>
+      <c r="H111">
+        <v>5.5</v>
+      </c>
+      <c r="I111">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A112" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" t="s">
+        <v>21</v>
+      </c>
+      <c r="C112" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" t="s">
+        <v>7</v>
+      </c>
+      <c r="F112">
+        <v>13.7</v>
+      </c>
+      <c r="G112">
+        <v>13.7</v>
+      </c>
+      <c r="H112">
+        <v>13.7</v>
+      </c>
+      <c r="I112">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A113" t="s">
+        <v>23</v>
+      </c>
+      <c r="B113" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" t="s">
+        <v>10</v>
+      </c>
+      <c r="E113" t="s">
+        <v>7</v>
+      </c>
+      <c r="F113">
+        <v>2.8</v>
+      </c>
+      <c r="G113">
+        <v>2.8</v>
+      </c>
+      <c r="H113">
+        <v>2.8</v>
+      </c>
+      <c r="I113">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A114" t="s">
+        <v>23</v>
+      </c>
+      <c r="B114" t="s">
+        <v>21</v>
+      </c>
+      <c r="C114" t="s">
+        <v>5</v>
+      </c>
+      <c r="D114" t="s">
+        <v>11</v>
+      </c>
+      <c r="E114" t="s">
+        <v>7</v>
+      </c>
+      <c r="F114">
+        <v>13.1</v>
+      </c>
+      <c r="G114">
+        <v>13.1</v>
+      </c>
+      <c r="H114">
+        <v>13.1</v>
+      </c>
+      <c r="I114">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A115" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" t="s">
+        <v>21</v>
+      </c>
+      <c r="C115" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115" t="s">
+        <v>7</v>
+      </c>
+      <c r="F115">
+        <v>36.4</v>
+      </c>
+      <c r="G115">
+        <v>36.4</v>
+      </c>
+      <c r="H115">
+        <v>36.4</v>
+      </c>
+      <c r="I115">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A116" t="s">
+        <v>23</v>
+      </c>
+      <c r="B116" t="s">
+        <v>52</v>
+      </c>
+      <c r="C116" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" t="s">
+        <v>7</v>
+      </c>
+      <c r="F116">
+        <v>21</v>
+      </c>
+      <c r="G116">
+        <v>21</v>
+      </c>
+      <c r="H116">
+        <v>21</v>
+      </c>
+      <c r="I116">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A117" t="s">
+        <v>23</v>
+      </c>
+      <c r="B117" t="s">
+        <v>52</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" t="s">
+        <v>7</v>
+      </c>
+      <c r="F117">
+        <v>10.9</v>
+      </c>
+      <c r="G117">
+        <v>10.9</v>
+      </c>
+      <c r="H117">
+        <v>10.9</v>
+      </c>
+      <c r="I117">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A118" t="s">
+        <v>23</v>
+      </c>
+      <c r="B118" t="s">
+        <v>52</v>
+      </c>
+      <c r="C118" t="s">
+        <v>5</v>
+      </c>
+      <c r="D118" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118">
+        <v>6.9</v>
+      </c>
+      <c r="G118">
+        <v>6.9</v>
+      </c>
+      <c r="H118">
+        <v>6.9</v>
+      </c>
+      <c r="I118">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A119" t="s">
+        <v>23</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C119" t="s">
+        <v>5</v>
+      </c>
+      <c r="D119" t="s">
+        <v>10</v>
+      </c>
+      <c r="E119" t="s">
+        <v>7</v>
+      </c>
+      <c r="F119">
+        <v>7.7</v>
+      </c>
+      <c r="G119">
+        <v>7.7</v>
+      </c>
+      <c r="H119">
+        <v>7.7</v>
+      </c>
+      <c r="I119">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A120" t="s">
+        <v>23</v>
+      </c>
+      <c r="B120" t="s">
+        <v>52</v>
+      </c>
+      <c r="C120" t="s">
+        <v>5</v>
+      </c>
+      <c r="D120" t="s">
+        <v>11</v>
+      </c>
+      <c r="E120" t="s">
+        <v>7</v>
+      </c>
+      <c r="F120">
+        <v>13.1</v>
+      </c>
+      <c r="G120">
+        <v>13.1</v>
+      </c>
+      <c r="H120">
+        <v>13.1</v>
+      </c>
+      <c r="I120">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A121" t="s">
+        <v>23</v>
+      </c>
+      <c r="B121" t="s">
+        <v>52</v>
+      </c>
+      <c r="C121" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="s">
+        <v>7</v>
+      </c>
+      <c r="F121">
+        <v>36.4</v>
+      </c>
+      <c r="G121">
+        <v>36.4</v>
+      </c>
+      <c r="H121">
+        <v>36.4</v>
+      </c>
+      <c r="I121">
+        <v>36.4</v>
       </c>
     </row>
   </sheetData>
@@ -2800,25 +4077,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98EC8B37-9B75-4E27-B572-3EA8EB4C7FF9}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="16.29296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.8203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -2838,16 +4116,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -2856,7 +4134,7 @@
         <v>6.4</v>
       </c>
       <c r="G2">
-        <v>6.8000000000000007</v>
+        <v>6.8</v>
       </c>
       <c r="H2">
         <v>7.2</v>
@@ -2864,25 +4142,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3">
-        <v>11.833333333333334</v>
+        <v>11.83</v>
       </c>
       <c r="G3">
-        <v>13.666666666666668</v>
+        <v>13.67</v>
       </c>
       <c r="H3">
         <v>15.5</v>
@@ -2890,45 +4168,45 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
       <c r="E4">
-        <v>2.4922126913209022</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="F4">
-        <v>6.392423028962817</v>
+        <v>6.39</v>
       </c>
       <c r="G4">
-        <v>5.8591337805562089</v>
+        <v>16.68</v>
       </c>
       <c r="H4">
-        <v>11.636545912491297</v>
+        <v>16.52</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
       <c r="E5">
-        <v>6.6101423872074365</v>
+        <v>6.61</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -2942,19 +4220,19 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
       <c r="E6">
-        <v>1.6902104760646837</v>
+        <v>1.69</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -2968,19 +4246,19 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
       <c r="E7">
-        <v>0.84510523803234183</v>
+        <v>0.85</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -2994,16 +4272,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3020,25 +4298,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
       <c r="E9">
-        <v>0.23827187566858199</v>
+        <v>0.24</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0.10473773754328589</v>
+        <v>1.17</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -3046,19 +4324,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
       <c r="E10">
-        <v>2.6257560698677733</v>
+        <v>2.63</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -3072,42 +4350,42 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
       <c r="E11">
-        <v>4.614988756343795</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="F11">
-        <v>15.497189968229545</v>
+        <v>15.5</v>
       </c>
       <c r="G11">
-        <v>14.005449897630072</v>
+        <v>1.95</v>
       </c>
       <c r="H11">
-        <v>11.112164629952847</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
-        <v>30</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3116,27 +4394,27 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0.52953898313082226</v>
+        <v>0.45</v>
       </c>
       <c r="H12">
-        <v>0.24636975015338317</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
       <c r="E13">
-        <v>2.5833125054944883</v>
+        <v>2.58</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -3150,42 +4428,42 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
         <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14">
-        <v>2.3437203361409713</v>
+        <v>2.34</v>
       </c>
       <c r="G14">
-        <v>6.267806267806268</v>
+        <v>6.27</v>
       </c>
       <c r="H14">
-        <v>6.3049197074024681</v>
+        <v>6.79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -3194,7 +4472,7 @@
         <v>6.4</v>
       </c>
       <c r="G15">
-        <v>6.8000000000000007</v>
+        <v>6.8</v>
       </c>
       <c r="H15">
         <v>7.2</v>
@@ -3202,25 +4480,25 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="F16">
-        <v>11.833333333333334</v>
+        <v>11.83</v>
       </c>
       <c r="G16">
-        <v>13.666666666666668</v>
+        <v>13.67</v>
       </c>
       <c r="H16">
         <v>15.5</v>
@@ -3228,48 +4506,48 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17">
-        <v>2.4922126913209022</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="F17">
-        <v>9.1723255418225307</v>
+        <v>9.17</v>
       </c>
       <c r="G17">
-        <v>8.9805158800981406</v>
+        <v>17.68</v>
       </c>
       <c r="H17">
-        <v>16.523599999999998</v>
+        <v>16.52</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18">
-        <v>6.6101423872074365</v>
+        <v>6.61</v>
       </c>
       <c r="F18">
-        <v>0.3524513535959477</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -3280,22 +4558,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E19">
-        <v>1.6902104760646837</v>
+        <v>1.69</v>
       </c>
       <c r="F19">
-        <v>8.3212720958024178E-2</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -3306,22 +4584,22 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20">
-        <v>0.84510523803234183</v>
+        <v>0.85</v>
       </c>
       <c r="F20">
-        <v>4.2527730316866158E-2</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3332,16 +4610,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -3358,25 +4636,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E22">
-        <v>0.23827187566858199</v>
+        <v>0.24</v>
       </c>
       <c r="F22">
-        <v>1.0149517989740465E-2</v>
+        <v>0.08</v>
       </c>
       <c r="G22">
-        <v>0.16053549048059779</v>
+        <v>1.17</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -3384,22 +4662,22 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E23">
-        <v>2.6257560698677733</v>
+        <v>2.63</v>
       </c>
       <c r="F23">
-        <v>0.34142637450283492</v>
+        <v>0.73</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -3410,71 +4688,71 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E24">
-        <v>4.614988756343795</v>
+        <v>4.6100000000000003</v>
       </c>
       <c r="F24">
-        <v>21.607999999999997</v>
+        <v>21.61</v>
       </c>
       <c r="G24">
-        <v>24.805779991511951</v>
+        <v>6.32</v>
       </c>
       <c r="H24">
-        <v>29.783999999999999</v>
+        <v>11.28</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25">
-        <v>2.7798498705794001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="G25">
-        <v>0.81164442138508863</v>
+        <v>0.69</v>
       </c>
       <c r="H25">
-        <v>0.28269938650306747</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E26">
-        <v>2.5833125054944883</v>
+        <v>2.58</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -3488,28 +4766,28 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>3.133903133903134</v>
+        <v>3.13</v>
       </c>
       <c r="G27">
-        <v>6.267806267806268</v>
+        <v>6.27</v>
       </c>
       <c r="H27">
-        <v>9.4017094017094021</v>
+        <v>9.4</v>
       </c>
     </row>
   </sheetData>
@@ -3518,15 +4796,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001B4ECEDC51D0484091AFD4177D66ED73" ma:contentTypeVersion="" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0cc653c178d9ffcb24786b6a9d53371f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b44fa922-a688-4301-8945-67f7597c9c55" xmlns:ns3="f6f44a7d-d6f5-4042-8792-19cb5f90fb06" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3af53c5407280ad7b07c166bc7f6511a" ns2:_="" ns3:_="">
     <xsd:import namespace="b44fa922-a688-4301-8945-67f7597c9c55"/>
@@ -3743,21 +5012,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33EE86CE-8AA5-48B2-94AD-241FD01903B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{772DCE14-3293-4B6E-AC91-8BC3FB109BAF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3776,11 +5046,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51F564AA-FEC3-44F3-A5AC-373F9783111F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33EE86CE-8AA5-48B2-94AD-241FD01903B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>